<commit_message>
change format of output files
</commit_message>
<xml_diff>
--- a/InstaData.xlsx
+++ b/InstaData.xlsx
@@ -11,14 +11,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+  <si>
+    <t>Creator Name</t>
+  </si>
+  <si>
+    <t>Area of Expertise</t>
   </si>
   <si>
     <t>Profession</t>
   </si>
   <si>
+    <t>Insta Handle</t>
+  </si>
+  <si>
     <t>Posts</t>
   </si>
   <si>
@@ -28,70 +34,142 @@
     <t>Following</t>
   </si>
   <si>
-    <t>InstaHandle</t>
-  </si>
-  <si>
     <t>Puja Kumar</t>
   </si>
   <si>
+    <t>art-and-craft</t>
+  </si>
+  <si>
     <t>Artist</t>
   </si>
   <si>
-    <t>740</t>
-  </si>
-  <si>
-    <t>8,837</t>
+    <t>artist_pujakumar</t>
+  </si>
+  <si>
+    <t>741</t>
+  </si>
+  <si>
+    <t>8,963</t>
   </si>
   <si>
     <t>412</t>
   </si>
   <si>
-    <t>artist_pujakumar</t>
-  </si>
-  <si>
     <t>Guin Srikanta</t>
   </si>
   <si>
-    <t>314</t>
-  </si>
-  <si>
-    <t>2,912</t>
-  </si>
-  <si>
-    <t>968</t>
-  </si>
-  <si>
     <t>guin_srikanta_watercolor</t>
   </si>
   <si>
+    <t>315</t>
+  </si>
+  <si>
+    <t>2,906</t>
+  </si>
+  <si>
+    <t>1,043</t>
+  </si>
+  <si>
     <t>Mahesh Honule</t>
   </si>
   <si>
+    <t>maheshhonule</t>
+  </si>
+  <si>
     <t>93</t>
   </si>
   <si>
-    <t>3,319</t>
+    <t>3,341</t>
   </si>
   <si>
     <t>221</t>
   </si>
   <si>
-    <t>maheshhonule</t>
-  </si>
-  <si>
     <t>Mahua Pal</t>
   </si>
   <si>
+    <t>mahua.pal.art</t>
+  </si>
+  <si>
     <t>265</t>
   </si>
   <si>
-    <t>10.1k</t>
-  </si>
-  <si>
-    <t>199</t>
-  </si>
-  <si>
-    <t>mahua.pal.art</t>
+    <t>10.2k</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Samir Mondal</t>
+  </si>
+  <si>
+    <t>samirmondal_watercolour</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>4,660</t>
+  </si>
+  <si>
+    <t>290</t>
+  </si>
+  <si>
+    <t>Sanjana Goenka</t>
+  </si>
+  <si>
+    <t>lineandcoconut</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>11.7k</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>Upasna Modi Poddar</t>
+  </si>
+  <si>
+    <t>oopsidoodledagain</t>
+  </si>
+  <si>
+    <t>492</t>
+  </si>
+  <si>
+    <t>3,400</t>
+  </si>
+  <si>
+    <t>824</t>
+  </si>
+  <si>
+    <t>The Killjoy Cat</t>
+  </si>
+  <si>
+    <t>thekilljoycat</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>1,107</t>
+  </si>
+  <si>
+    <t>610</t>
+  </si>
+  <si>
+    <t>| Uncle Subbu Comics |</t>
+  </si>
+  <si>
+    <t>unclesubbucomics</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
+    <t>385</t>
   </si>
 </sst>
 </file>
@@ -131,13 +209,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -156,85 +234,215 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>22</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
capitalize first letter of every word in Area of Expertise
</commit_message>
<xml_diff>
--- a/InstaData.xlsx
+++ b/InstaData.xlsx
@@ -40,7 +40,7 @@
     <t>Puja Kumar</t>
   </si>
   <si>
-    <t>art-and-craft</t>
+    <t>Art And Craft</t>
   </si>
   <si>
     <t>Artist</t>
@@ -166,8 +166,7 @@
     <t>610</t>
   </si>
   <si>
-    <t>thekilljoycat@gmail.com
-</t>
+    <t>thekilljoycat@gmail.com</t>
   </si>
   <si>
     <t>| Uncle Subbu Comics |</t>
@@ -290,8 +289,7 @@
     <t>450</t>
   </si>
   <si>
-    <t>postoncards@gmail.com
-</t>
+    <t>postoncards@gmail.com</t>
   </si>
   <si>
     <t>Nidhika-Holistic Health Coach</t>
@@ -570,8 +568,7 @@
     <t>529</t>
   </si>
   <si>
-    <t>artdesk.saara@gmail.comCommissions
-</t>
+    <t>artdesk.saara@gmail.comCommissions</t>
   </si>
   <si>
     <t>Amit Kapoor</t>
@@ -664,8 +661,7 @@
     <t>2,184</t>
   </si>
   <si>
-    <t>commissionsamirkhanpathanstudio@gmail.com
-</t>
+    <t>commissionsamirkhanpathanstudio@gmail.com</t>
   </si>
   <si>
     <t>Ravi Shankar</t>
@@ -716,7 +712,7 @@
     <t>Poonam Sapra</t>
   </si>
   <si>
-    <t>creators</t>
+    <t>Creators</t>
   </si>
   <si>
     <t>motherwithsign</t>
@@ -764,8 +760,7 @@
     <t>85</t>
   </si>
   <si>
-    <t>ageisjustanumber62@gmail.com
-</t>
+    <t>ageisjustanumber62@gmail.com</t>
   </si>
   <si>
     <t>Padma Balasubramanian</t>
@@ -801,14 +796,13 @@
     <t>17</t>
   </si>
   <si>
-    <t>d@vasantiakhani2.0
-</t>
+    <t>d@vasantiakhani2.0</t>
   </si>
   <si>
     <t>Ishpreet (Isha)</t>
   </si>
   <si>
-    <t>dance</t>
+    <t>Dance</t>
   </si>
   <si>
     <t>ishpreet_dang</t>
@@ -823,14 +817,13 @@
     <t>969</t>
   </si>
   <si>
-    <t>Collab-mailishadang@gmail.comTutorials
-</t>
+    <t>Collab-mailishadang@gmail.comTutorials</t>
   </si>
   <si>
     <t>Saurav Sinha</t>
   </si>
   <si>
-    <t>photography</t>
+    <t>Photography</t>
   </si>
   <si>
     <t>sauravus</t>
@@ -875,8 +868,7 @@
     <t>162</t>
   </si>
   <si>
-    <t>reach.nishchay@gmail.com
-</t>
+    <t>reach.nishchay@gmail.com</t>
   </si>
   <si>
     <t>Sumeet  🇮🇳</t>
@@ -1038,8 +1030,7 @@
     <t>405</t>
   </si>
   <si>
-    <t>Sudhir@SudhirShivaram.com
-</t>
+    <t>Sudhir@SudhirShivaram.com</t>
   </si>
   <si>
     <t>Priyanshi</t>
@@ -1129,8 +1120,7 @@
     <t>68k</t>
   </si>
   <si>
-    <t>Kushagra@exifmedia.comCreative
-</t>
+    <t>Kushagra@exifmedia.comCreative</t>
   </si>
   <si>
     <t>ANUNAY SOOD | India 🇮🇳</t>
@@ -1163,8 +1153,7 @@
     <t>834</t>
   </si>
   <si>
-    <t>ajinkyakalbhor59@gmail.com
-</t>
+    <t>ajinkyakalbhor59@gmail.com</t>
   </si>
   <si>
     <t>Harshall | INDIA</t>
@@ -1212,8 +1201,7 @@
     <t>307</t>
   </si>
   <si>
-    <t>Ulachhiramka@gmail.com
-</t>
+    <t>Ulachhiramka@gmail.com</t>
   </si>
   <si>
     <t>Pankaj Prajapati | India 🇮🇳</t>
@@ -1231,8 +1219,7 @@
     <t>428</t>
   </si>
   <si>
-    <t>snapwithpankaj@gmail.com
-</t>
+    <t>snapwithpankaj@gmail.com</t>
   </si>
   <si>
     <t>Abhishek</t>
@@ -1415,8 +1402,7 @@
     <t>724</t>
   </si>
   <si>
-    <t>subhashs.in@gmail.com
-</t>
+    <t>subhashs.in@gmail.com</t>
   </si>
   <si>
     <t>aarzoo_khurana_photography</t>
@@ -1641,8 +1627,7 @@
     <t>984</t>
   </si>
   <si>
-    <t>kunalmalhotrakunal.malhotra2604@gmail.comLEARN
-</t>
+    <t>kunalmalhotrakunal.malhotra2604@gmail.comLEARN</t>
   </si>
   <si>
     <t>Roshani Shah | INDIA</t>
@@ -1660,8 +1645,7 @@
     <t>706</t>
   </si>
   <si>
-    <t>roshanishah181@gmail.com
-</t>
+    <t>roshanishah181@gmail.com</t>
   </si>
   <si>
     <t>Prakriti Maurya | Delhi</t>
@@ -1682,7 +1666,7 @@
     <t>S A M E E R   O B E R O I</t>
   </si>
   <si>
-    <t>poetry</t>
+    <t>Poetry</t>
   </si>
   <si>
     <t>thesameeroberoi</t>
@@ -1916,14 +1900,13 @@
     <t>23</t>
   </si>
   <si>
-    <t>kopal@tapeatale.com
-</t>
+    <t>kopal@tapeatale.com</t>
   </si>
   <si>
     <t>dinesh mohan silverfox India</t>
   </si>
   <si>
-    <t>theatre-drama</t>
+    <t>Theatre Drama</t>
   </si>
   <si>
     <t>Actor</t>

</xml_diff>